<commit_message>
updated meeting notes with info about merging sample info into the variant csv
</commit_message>
<xml_diff>
--- a/sample_info/DGETesselatusTissues2022.xlsx
+++ b/sample_info/DGETesselatusTissues2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tss0019/Library/CloudStorage/Box-Box/SchwartzLab/Projects/TS_Lab_Whiptails/2022_ASE_Klabacka/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dixiestate-my.sharepoint.com/personal/d00498331_utahtech_edu/Documents/KLab/Research/2023_WhiptailNmtVariation/whiptail_dge_tissues/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1A53E0-1439-D542-A0EF-3F4DBA38548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1B1A53E0-1439-D542-A0EF-3F4DBA38548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1B63760-E5F4-5E4F-B7EE-071BBBD644D4}"/>
   <bookViews>
-    <workbookView xWindow="19820" yWindow="6040" windowWidth="25300" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="760" windowWidth="29380" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSpreadsheet_June2019" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>RLK063</t>
   </si>
   <si>
-    <t>Sequence_ID</t>
-  </si>
-  <si>
     <t>Am_01</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>SampleID</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -881,7 +881,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -941,9 +940,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -981,7 +980,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1087,7 +1086,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1229,7 +1228,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2014,7 +2013,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2024,7 +2023,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>70</v>
@@ -2033,12 +2032,12 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -2055,7 +2054,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
@@ -2072,7 +2071,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -2089,7 +2088,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>25</v>
@@ -2106,7 +2105,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>25</v>
@@ -2123,7 +2122,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>25</v>
@@ -2140,7 +2139,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>28</v>
@@ -2157,7 +2156,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>28</v>
@@ -2174,7 +2173,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>28</v>
@@ -2191,7 +2190,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>29</v>
@@ -2208,7 +2207,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>29</v>
@@ -2225,7 +2224,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>29</v>
@@ -2242,7 +2241,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>75</v>
@@ -2253,7 +2252,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>75</v>
@@ -2264,7 +2263,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>75</v>
@@ -2275,12 +2274,12 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
@@ -2292,7 +2291,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>37</v>
@@ -2309,7 +2308,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>38</v>
@@ -2326,7 +2325,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>40</v>
@@ -2343,7 +2342,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>41</v>
@@ -2360,7 +2359,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>42</v>
@@ -2377,7 +2376,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>48</v>
@@ -2394,7 +2393,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>49</v>
@@ -2411,7 +2410,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>53</v>
@@ -2428,7 +2427,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>23</v>
@@ -2445,7 +2444,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>23</v>
@@ -2462,7 +2461,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>23</v>

</xml_diff>